<commit_message>
minor fix for template.xlsx
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-22.04\home\yamamoto\public\kst-txg\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54388542-6069-43EB-A5BB-53FEDF9D0656}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E6C4A7A-E4F4-47B0-AE0C-DE330E3B6A9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" tabRatio="654" activeTab="1" xr2:uid="{17B2CA72-8830-438C-B688-BD9A9A7A95FD}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" tabRatio="654" activeTab="4" xr2:uid="{17B2CA72-8830-438C-B688-BD9A9A7A95FD}"/>
   </bookViews>
   <sheets>
     <sheet name="学外研究・学会活動届" sheetId="3" r:id="rId1"/>
@@ -3813,9 +3813,6 @@
     <phoneticPr fontId="4"/>
   </si>
   <si>
-    <t>プルダウンで選択</t>
-  </si>
-  <si>
     <t>円</t>
     <rPh sb="0" eb="1">
       <t>エン</t>
@@ -4750,6 +4747,9 @@
   <si>
     <t>##%資金名・資金コード##</t>
     <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>（２）銀行振込</t>
   </si>
 </sst>
 </file>
@@ -6406,7 +6406,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="715">
+  <cellXfs count="716">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -8444,6 +8444,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="53" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="53" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -10019,7 +10022,7 @@
       <c r="AO1" s="165"/>
       <c r="AP1" s="165"/>
       <c r="AQ1" s="256" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="AR1" s="256"/>
       <c r="AS1" s="256"/>
@@ -10283,7 +10286,7 @@
       <c r="E6" s="203"/>
       <c r="F6" s="203"/>
       <c r="G6" s="265" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="H6" s="263"/>
       <c r="I6" s="263"/>
@@ -10297,12 +10300,12 @@
       <c r="Q6" s="263"/>
       <c r="R6" s="263"/>
       <c r="S6" s="263" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="T6" s="263"/>
       <c r="U6" s="264"/>
       <c r="V6" s="266" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="W6" s="266"/>
       <c r="X6" s="266"/>
@@ -10319,7 +10322,7 @@
       <c r="AE6" s="203"/>
       <c r="AF6" s="203"/>
       <c r="AG6" s="270" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="AH6" s="266"/>
       <c r="AI6" s="266"/>
@@ -10355,7 +10358,7 @@
       <c r="E7" s="201"/>
       <c r="F7" s="201"/>
       <c r="G7" s="260" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="H7" s="260"/>
       <c r="I7" s="260"/>
@@ -10385,7 +10388,7 @@
       <c r="AE7" s="201"/>
       <c r="AF7" s="201"/>
       <c r="AG7" s="211" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="AH7" s="211"/>
       <c r="AI7" s="211"/>
@@ -10421,7 +10424,7 @@
       <c r="E8" s="201"/>
       <c r="F8" s="201"/>
       <c r="G8" s="235" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="H8" s="236"/>
       <c r="I8" s="236"/>
@@ -10451,7 +10454,7 @@
       <c r="AE8" s="208"/>
       <c r="AF8" s="209"/>
       <c r="AG8" s="211" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="AH8" s="211"/>
       <c r="AI8" s="211"/>
@@ -10495,7 +10498,7 @@
       <c r="M9" s="234"/>
       <c r="N9" s="234"/>
       <c r="O9" s="258" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="P9" s="259"/>
       <c r="Q9" s="204" t="s">
@@ -10510,7 +10513,7 @@
       <c r="X9" s="204"/>
       <c r="Y9" s="205"/>
       <c r="Z9" s="258" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="AA9" s="259"/>
       <c r="AB9" s="232" t="s">
@@ -10671,7 +10674,7 @@
     </row>
     <row r="12" spans="1:56" ht="50.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A12" s="250" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B12" s="211"/>
       <c r="C12" s="211"/>
@@ -10699,7 +10702,7 @@
       <c r="Y12" s="211"/>
       <c r="Z12" s="211"/>
       <c r="AA12" s="155" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="AB12" s="156"/>
       <c r="AC12" s="156"/>
@@ -10793,7 +10796,7 @@
     </row>
     <row r="14" spans="1:56" ht="60" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A14" s="166" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B14" s="167"/>
       <c r="C14" s="167"/>
@@ -10861,7 +10864,7 @@
       <c r="E15" s="159"/>
       <c r="F15" s="159"/>
       <c r="G15" s="160" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="H15" s="161"/>
       <c r="I15" s="161"/>
@@ -10875,7 +10878,7 @@
       </c>
       <c r="P15" s="199"/>
       <c r="Q15" s="161" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="R15" s="161"/>
       <c r="S15" s="161"/>
@@ -10884,7 +10887,7 @@
       </c>
       <c r="U15" s="199"/>
       <c r="V15" s="161" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="W15" s="161"/>
       <c r="X15" s="161"/>
@@ -10897,7 +10900,7 @@
       </c>
       <c r="AB15" s="199"/>
       <c r="AC15" s="161" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="AD15" s="161"/>
       <c r="AE15" s="161"/>
@@ -10907,7 +10910,7 @@
       </c>
       <c r="AH15" s="199"/>
       <c r="AI15" s="161" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="AJ15" s="161"/>
       <c r="AK15" s="161"/>
@@ -10916,7 +10919,7 @@
       </c>
       <c r="AM15" s="199"/>
       <c r="AN15" s="161" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="AO15" s="161"/>
       <c r="AP15" s="161"/>
@@ -11009,7 +11012,7 @@
       <c r="E17" s="176"/>
       <c r="F17" s="176"/>
       <c r="G17" s="177" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="H17" s="178"/>
       <c r="I17" s="179" t="s">
@@ -11023,7 +11026,7 @@
       <c r="O17" s="180"/>
       <c r="P17" s="181"/>
       <c r="Q17" s="182" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="R17" s="182"/>
       <c r="S17" s="183" t="s">
@@ -11044,7 +11047,7 @@
       <c r="AD17" s="252"/>
       <c r="AE17" s="253"/>
       <c r="AF17" s="196" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="AG17" s="197"/>
       <c r="AH17" s="197"/>
@@ -11091,7 +11094,7 @@
       <c r="O18" s="191"/>
       <c r="P18" s="192"/>
       <c r="Q18" s="222" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="R18" s="215"/>
       <c r="S18" s="216" t="s">
@@ -11105,7 +11108,7 @@
       <c r="Y18" s="216"/>
       <c r="Z18" s="216"/>
       <c r="AA18" s="215" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="AB18" s="215"/>
       <c r="AC18" s="216" t="s">
@@ -11405,7 +11408,7 @@
       <c r="T23" s="242"/>
       <c r="U23" s="243"/>
       <c r="V23" s="185" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="W23" s="186"/>
       <c r="X23" s="186"/>
@@ -11728,7 +11731,7 @@
   </sheetPr>
   <dimension ref="A1:BK69"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="L14" sqref="L14:AD15"/>
     </sheetView>
   </sheetViews>
@@ -11891,7 +11894,7 @@
       <c r="Y6" s="279"/>
       <c r="Z6" s="279"/>
       <c r="AA6" s="280" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="AB6" s="280"/>
       <c r="AC6" s="280"/>
@@ -11987,7 +11990,7 @@
       </c>
       <c r="G8" s="294"/>
       <c r="H8" s="295" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="I8" s="296"/>
       <c r="J8" s="296"/>
@@ -12009,7 +12012,7 @@
       <c r="X8" s="299"/>
       <c r="Y8" s="299"/>
       <c r="Z8" s="300" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="AA8" s="301"/>
       <c r="AB8" s="301"/>
@@ -12030,7 +12033,7 @@
       </c>
       <c r="G9" s="304"/>
       <c r="H9" s="305" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="I9" s="306"/>
       <c r="J9" s="306"/>
@@ -12075,7 +12078,7 @@
       </c>
       <c r="G10" s="314"/>
       <c r="H10" s="315" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="I10" s="316"/>
       <c r="J10" s="316"/>
@@ -12097,7 +12100,7 @@
       <c r="V10" s="318"/>
       <c r="W10" s="318"/>
       <c r="X10" s="319" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="Y10" s="319"/>
       <c r="Z10" s="319"/>
@@ -12122,7 +12125,7 @@
       </c>
       <c r="G11" s="331"/>
       <c r="H11" s="332" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="I11" s="333"/>
       <c r="J11" s="333"/>
@@ -12163,7 +12166,7 @@
       </c>
       <c r="G12" s="304"/>
       <c r="H12" s="305" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="I12" s="306"/>
       <c r="J12" s="306"/>
@@ -12208,7 +12211,7 @@
       </c>
       <c r="G13" s="314"/>
       <c r="H13" s="315" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="I13" s="316"/>
       <c r="J13" s="316"/>
@@ -12230,7 +12233,7 @@
       <c r="V13" s="318"/>
       <c r="W13" s="318"/>
       <c r="X13" s="319" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="Y13" s="319"/>
       <c r="Z13" s="319"/>
@@ -12259,7 +12262,7 @@
       <c r="J14" s="342"/>
       <c r="K14" s="343"/>
       <c r="L14" s="345" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="M14" s="346"/>
       <c r="N14" s="346"/>
@@ -12327,7 +12330,7 @@
       <c r="D16" s="186"/>
       <c r="E16" s="247"/>
       <c r="F16" s="310" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="G16" s="311"/>
       <c r="H16" s="311"/>
@@ -12338,7 +12341,7 @@
         <v>85</v>
       </c>
       <c r="M16" s="311" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="N16" s="311"/>
       <c r="O16" s="311"/>
@@ -12349,7 +12352,7 @@
         <v>48</v>
       </c>
       <c r="T16" s="312" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="U16" s="312"/>
       <c r="V16" s="113" t="s">
@@ -12376,7 +12379,7 @@
       <c r="D17" s="186"/>
       <c r="E17" s="247"/>
       <c r="F17" s="351" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="G17" s="352"/>
       <c r="H17" s="352"/>
@@ -12506,7 +12509,7 @@
       </c>
       <c r="L20" s="366"/>
       <c r="M20" s="366" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="N20" s="366"/>
       <c r="O20" s="366"/>
@@ -12518,7 +12521,7 @@
       </c>
       <c r="T20" s="375"/>
       <c r="U20" s="375" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="V20" s="375"/>
       <c r="W20" s="375"/>
@@ -12547,7 +12550,7 @@
       <c r="I21" s="363"/>
       <c r="J21" s="364"/>
       <c r="K21" s="382" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="L21" s="383"/>
       <c r="M21" s="383"/>
@@ -12559,7 +12562,7 @@
       </c>
       <c r="R21" s="384"/>
       <c r="S21" s="382" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="T21" s="383"/>
       <c r="U21" s="383"/>
@@ -12598,33 +12601,33 @@
       <c r="M22" s="386"/>
       <c r="N22" s="386"/>
       <c r="O22" s="387" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="P22" s="388"/>
       <c r="Q22" s="185" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="R22" s="247"/>
       <c r="S22" s="185" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="T22" s="247"/>
       <c r="U22" s="185" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="V22" s="247"/>
       <c r="W22" s="185" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="X22" s="186"/>
       <c r="Y22" s="186"/>
       <c r="Z22" s="247"/>
       <c r="AA22" s="185" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="AB22" s="247"/>
       <c r="AC22" s="185" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="AD22" s="389"/>
       <c r="AF22" s="57" t="s">
@@ -12649,7 +12652,7 @@
       <c r="M23" s="386"/>
       <c r="N23" s="386"/>
       <c r="O23" s="390" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="P23" s="391"/>
       <c r="Q23" s="391"/>
@@ -12688,7 +12691,7 @@
       <c r="M24" s="386"/>
       <c r="N24" s="386"/>
       <c r="O24" s="424" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="P24" s="425"/>
       <c r="Q24" s="425"/>
@@ -13014,15 +13017,15 @@
     </row>
     <row r="32" spans="1:32" s="16" customFormat="1" ht="26.45" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A32" s="438" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B32" s="387"/>
       <c r="C32" s="387" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="D32" s="387"/>
       <c r="E32" s="439" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="F32" s="440"/>
       <c r="G32" s="440"/>
@@ -13055,15 +13058,15 @@
     </row>
     <row r="33" spans="1:32" s="16" customFormat="1" ht="26.45" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A33" s="442" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B33" s="443"/>
       <c r="C33" s="185" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="D33" s="247"/>
       <c r="E33" s="439" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="F33" s="440"/>
       <c r="G33" s="440"/>
@@ -13096,15 +13099,15 @@
     </row>
     <row r="34" spans="1:32" s="16" customFormat="1" ht="26.45" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A34" s="442" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B34" s="443"/>
       <c r="C34" s="185" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="D34" s="247"/>
       <c r="E34" s="439" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="F34" s="440"/>
       <c r="G34" s="440"/>
@@ -13134,15 +13137,15 @@
     </row>
     <row r="35" spans="1:32" s="16" customFormat="1" ht="26.45" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A35" s="438" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B35" s="387"/>
       <c r="C35" s="387" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="D35" s="387"/>
       <c r="E35" s="439" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="F35" s="440"/>
       <c r="G35" s="440"/>
@@ -13175,15 +13178,15 @@
     </row>
     <row r="36" spans="1:32" s="16" customFormat="1" ht="26.45" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A36" s="442" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B36" s="443"/>
       <c r="C36" s="185" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="D36" s="247"/>
       <c r="E36" s="439" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="F36" s="440"/>
       <c r="G36" s="440"/>
@@ -13213,15 +13216,15 @@
     </row>
     <row r="37" spans="1:32" s="16" customFormat="1" ht="26.45" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A37" s="442" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B37" s="443"/>
       <c r="C37" s="185" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D37" s="247"/>
       <c r="E37" s="439" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="F37" s="440"/>
       <c r="G37" s="440"/>
@@ -13251,15 +13254,15 @@
     </row>
     <row r="38" spans="1:32" s="16" customFormat="1" ht="26.45" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A38" s="442" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B38" s="443"/>
       <c r="C38" s="185" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="D38" s="247"/>
       <c r="E38" s="439" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="F38" s="440"/>
       <c r="G38" s="440"/>
@@ -13289,15 +13292,15 @@
     </row>
     <row r="39" spans="1:32" s="16" customFormat="1" ht="26.45" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A39" s="442" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B39" s="443"/>
       <c r="C39" s="185" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="D39" s="247"/>
       <c r="E39" s="439" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="F39" s="440"/>
       <c r="G39" s="440"/>
@@ -13327,15 +13330,15 @@
     </row>
     <row r="40" spans="1:32" s="16" customFormat="1" ht="26.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A40" s="438" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B40" s="387"/>
       <c r="C40" s="387" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="D40" s="387"/>
       <c r="E40" s="439" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="F40" s="440"/>
       <c r="G40" s="440"/>
@@ -13502,7 +13505,7 @@
       <c r="C44" s="471"/>
       <c r="D44" s="472"/>
       <c r="E44" s="473" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="F44" s="474"/>
       <c r="G44" s="474"/>
@@ -14610,7 +14613,7 @@
       </c>
       <c r="S3" s="551"/>
       <c r="T3" s="552" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="U3" s="552"/>
       <c r="V3" s="552"/>
@@ -14634,7 +14637,7 @@
     </row>
     <row r="5" spans="1:33" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="553" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="B5" s="553"/>
       <c r="C5" s="553"/>
@@ -14687,7 +14690,7 @@
       <c r="R7" s="486"/>
       <c r="S7" s="486"/>
       <c r="T7" s="490" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="U7" s="490"/>
       <c r="V7" s="490"/>
@@ -14709,7 +14712,7 @@
       <c r="R8" s="487"/>
       <c r="S8" s="487"/>
       <c r="T8" s="556" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="U8" s="556"/>
       <c r="V8" s="556"/>
@@ -14879,7 +14882,7 @@
       </c>
       <c r="G14" s="387"/>
       <c r="H14" s="565" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="I14" s="566"/>
       <c r="J14" s="566"/>
@@ -14918,7 +14921,7 @@
       </c>
       <c r="G15" s="387"/>
       <c r="H15" s="510" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="I15" s="511"/>
       <c r="J15" s="511"/>
@@ -14960,7 +14963,7 @@
       </c>
       <c r="G16" s="339"/>
       <c r="H16" s="542" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="I16" s="543"/>
       <c r="J16" s="543"/>
@@ -15032,7 +15035,7 @@
       <c r="D18" s="504"/>
       <c r="E18" s="505"/>
       <c r="F18" s="506" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="G18" s="507"/>
       <c r="H18" s="507"/>
@@ -15043,7 +15046,7 @@
         <v>85</v>
       </c>
       <c r="M18" s="507" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="N18" s="507"/>
       <c r="O18" s="507"/>
@@ -15054,7 +15057,7 @@
         <v>48</v>
       </c>
       <c r="T18" s="508" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="U18" s="508"/>
       <c r="V18" s="59" t="s">
@@ -15081,7 +15084,7 @@
       <c r="D19" s="504"/>
       <c r="E19" s="505"/>
       <c r="F19" s="558" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="G19" s="559"/>
       <c r="H19" s="559"/>
@@ -15120,7 +15123,7 @@
       <c r="D20" s="504"/>
       <c r="E20" s="505"/>
       <c r="F20" s="513" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="G20" s="354"/>
       <c r="H20" s="354"/>
@@ -15159,7 +15162,7 @@
       <c r="D21" s="516"/>
       <c r="E21" s="517"/>
       <c r="F21" s="521" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="G21" s="522"/>
       <c r="H21" s="522"/>
@@ -15239,7 +15242,7 @@
       </c>
       <c r="G23" s="247"/>
       <c r="H23" s="537" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="I23" s="538"/>
       <c r="J23" s="538"/>
@@ -15278,7 +15281,7 @@
       </c>
       <c r="G24" s="387"/>
       <c r="H24" s="510" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="I24" s="511"/>
       <c r="J24" s="511"/>
@@ -15320,7 +15323,7 @@
       </c>
       <c r="G25" s="339"/>
       <c r="H25" s="491" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="I25" s="492"/>
       <c r="J25" s="492"/>
@@ -15392,14 +15395,14 @@
       <c r="E27" s="570"/>
       <c r="F27" s="51"/>
       <c r="G27" s="540" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="H27" s="540"/>
       <c r="I27" s="50" t="s">
         <v>109</v>
       </c>
       <c r="J27" s="496" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="K27" s="496"/>
       <c r="L27" s="496"/>
@@ -15414,7 +15417,7 @@
       <c r="S27" s="496"/>
       <c r="T27" s="497"/>
       <c r="U27" s="499" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="V27" s="500"/>
       <c r="W27" s="500"/>
@@ -15807,7 +15810,7 @@
       <c r="A3" s="6"/>
       <c r="B3" s="6"/>
       <c r="C3" s="495" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="D3" s="495"/>
       <c r="E3" s="495"/>
@@ -15835,7 +15838,7 @@
       <c r="Y3" s="39"/>
       <c r="Z3" s="39"/>
       <c r="AA3" s="637" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="AB3" s="637"/>
       <c r="AC3" s="637"/>
@@ -15965,7 +15968,7 @@
       <c r="AA6" s="6"/>
       <c r="AB6" s="6"/>
       <c r="AC6" s="628" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="AD6" s="628"/>
       <c r="AE6" s="628"/>
@@ -16120,7 +16123,7 @@
         <v>48</v>
       </c>
       <c r="H10" s="555" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="I10" s="555"/>
       <c r="J10" s="555"/>
@@ -16145,7 +16148,7 @@
       <c r="AA10" s="6"/>
       <c r="AB10" s="6"/>
       <c r="AC10" s="555" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="AD10" s="555"/>
       <c r="AE10" s="555"/>
@@ -16215,7 +16218,7 @@
       <c r="Y12" s="577"/>
       <c r="Z12" s="577"/>
       <c r="AA12" s="631" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="AB12" s="631"/>
       <c r="AC12" s="631"/>
@@ -16225,7 +16228,7 @@
       </c>
       <c r="AF12" s="577"/>
       <c r="AG12" s="631" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="AH12" s="631"/>
       <c r="AI12" s="632"/>
@@ -16279,7 +16282,7 @@
       </c>
       <c r="D14" s="517"/>
       <c r="E14" s="586" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="F14" s="587"/>
       <c r="G14" s="587"/>
@@ -16290,7 +16293,7 @@
       </c>
       <c r="K14" s="66"/>
       <c r="L14" s="586" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="M14" s="587"/>
       <c r="N14" s="587"/>
@@ -16356,28 +16359,28 @@
       <c r="C16" s="562"/>
       <c r="D16" s="564"/>
       <c r="E16" s="154" t="s">
+        <v>396</v>
+      </c>
+      <c r="F16" s="154" t="s">
         <v>397</v>
       </c>
-      <c r="F16" s="154" t="s">
+      <c r="G16" s="154" t="s">
         <v>398</v>
       </c>
-      <c r="G16" s="154" t="s">
+      <c r="H16" s="154" t="s">
         <v>399</v>
       </c>
-      <c r="H16" s="154" t="s">
+      <c r="I16" s="154" t="s">
         <v>400</v>
       </c>
-      <c r="I16" s="154" t="s">
+      <c r="J16" s="154" t="s">
         <v>401</v>
       </c>
-      <c r="J16" s="154" t="s">
+      <c r="K16" s="154" t="s">
         <v>402</v>
       </c>
-      <c r="K16" s="154" t="s">
+      <c r="L16" s="586" t="s">
         <v>403</v>
-      </c>
-      <c r="L16" s="586" t="s">
-        <v>404</v>
       </c>
       <c r="M16" s="587"/>
       <c r="N16" s="587"/>
@@ -16399,7 +16402,7 @@
       <c r="AC16" s="580"/>
       <c r="AD16" s="21"/>
       <c r="AE16" s="636" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="AF16" s="636"/>
       <c r="AG16" s="636"/>
@@ -16518,7 +16521,7 @@
     </row>
     <row r="21" spans="1:36" ht="21" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B21" s="599" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="C21" s="306"/>
       <c r="D21" s="306"/>
@@ -16535,17 +16538,17 @@
       <c r="O21" s="306"/>
       <c r="P21" s="600"/>
       <c r="Q21" s="601" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="R21" s="602"/>
       <c r="S21" s="603" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="T21" s="604"/>
       <c r="U21" s="604"/>
       <c r="V21" s="605"/>
       <c r="W21" s="606" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="X21" s="607"/>
       <c r="Y21" s="607"/>
@@ -16562,7 +16565,7 @@
     </row>
     <row r="22" spans="1:36" ht="21" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B22" s="599" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="C22" s="306"/>
       <c r="D22" s="306"/>
@@ -16579,17 +16582,17 @@
       <c r="O22" s="306"/>
       <c r="P22" s="600"/>
       <c r="Q22" s="601" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="R22" s="602"/>
       <c r="S22" s="603" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="T22" s="604"/>
       <c r="U22" s="604"/>
       <c r="V22" s="605"/>
       <c r="W22" s="606" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="X22" s="607"/>
       <c r="Y22" s="607"/>
@@ -16606,7 +16609,7 @@
     </row>
     <row r="23" spans="1:36" ht="21" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B23" s="599" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="C23" s="306"/>
       <c r="D23" s="306"/>
@@ -16623,17 +16626,17 @@
       <c r="O23" s="306"/>
       <c r="P23" s="600"/>
       <c r="Q23" s="601" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="R23" s="602"/>
       <c r="S23" s="603" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="T23" s="604"/>
       <c r="U23" s="604"/>
       <c r="V23" s="605"/>
       <c r="W23" s="606" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="X23" s="607"/>
       <c r="Y23" s="607"/>
@@ -16650,7 +16653,7 @@
     </row>
     <row r="24" spans="1:36" ht="21" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B24" s="599" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="C24" s="306"/>
       <c r="D24" s="306"/>
@@ -16667,17 +16670,17 @@
       <c r="O24" s="306"/>
       <c r="P24" s="600"/>
       <c r="Q24" s="601" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="R24" s="602"/>
       <c r="S24" s="603" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="T24" s="604"/>
       <c r="U24" s="604"/>
       <c r="V24" s="605"/>
       <c r="W24" s="606" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="X24" s="607"/>
       <c r="Y24" s="607"/>
@@ -16694,7 +16697,7 @@
     </row>
     <row r="25" spans="1:36" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B25" s="609" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="C25" s="610"/>
       <c r="D25" s="610"/>
@@ -16711,17 +16714,17 @@
       <c r="O25" s="610"/>
       <c r="P25" s="611"/>
       <c r="Q25" s="612" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="R25" s="613"/>
       <c r="S25" s="614" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="T25" s="615"/>
       <c r="U25" s="615"/>
       <c r="V25" s="616"/>
       <c r="W25" s="617" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="X25" s="618"/>
       <c r="Y25" s="618"/>
@@ -17568,8 +17571,8 @@
   </sheetPr>
   <dimension ref="A1:AF43"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="M12" sqref="M12:AD12"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A3" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15:AD15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.4"/>
@@ -17615,7 +17618,7 @@
       <c r="U1" s="273"/>
       <c r="V1" s="273"/>
       <c r="W1" s="275" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="X1" s="273"/>
       <c r="Y1" s="273"/>
@@ -17692,11 +17695,11 @@
     </row>
     <row r="4" spans="1:32" ht="24" customHeight="1" x14ac:dyDescent="0.4">
       <c r="U4" s="273" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="V4" s="273"/>
       <c r="W4" s="273" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="X4" s="273"/>
       <c r="Y4" s="273"/>
@@ -17709,7 +17712,7 @@
     </row>
     <row r="5" spans="1:32" ht="30.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A5" s="712" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B5" s="712"/>
       <c r="C5" s="712"/>
@@ -17744,7 +17747,7 @@
     </row>
     <row r="6" spans="1:32" ht="23.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A6" s="641" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B6" s="387"/>
       <c r="C6" s="387"/>
@@ -17755,7 +17758,7 @@
       </c>
       <c r="G6" s="386"/>
       <c r="H6" s="692" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="I6" s="693"/>
       <c r="J6" s="693"/>
@@ -17769,7 +17772,7 @@
       <c r="R6" s="693"/>
       <c r="S6" s="694"/>
       <c r="T6" s="695" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="U6" s="664"/>
       <c r="V6" s="664"/>
@@ -17777,12 +17780,12 @@
       <c r="X6" s="664"/>
       <c r="Y6" s="664"/>
       <c r="Z6" s="713" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="AA6" s="714"/>
       <c r="AB6" s="714"/>
       <c r="AC6" s="714"/>
-      <c r="AD6" s="714"/>
+      <c r="AD6" s="715"/>
       <c r="AF6" s="57"/>
     </row>
     <row r="7" spans="1:32" ht="23.25" customHeight="1" x14ac:dyDescent="0.4">
@@ -17796,7 +17799,7 @@
       </c>
       <c r="G7" s="386"/>
       <c r="H7" s="697" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="I7" s="698"/>
       <c r="J7" s="698"/>
@@ -17833,7 +17836,7 @@
       </c>
       <c r="G8" s="386"/>
       <c r="H8" s="692" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="I8" s="693"/>
       <c r="J8" s="693"/>
@@ -17855,7 +17858,7 @@
       <c r="V8" s="695"/>
       <c r="W8" s="695"/>
       <c r="X8" s="692" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="Y8" s="693"/>
       <c r="Z8" s="693"/>
@@ -17867,7 +17870,7 @@
     </row>
     <row r="9" spans="1:32" ht="23.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A9" s="663" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B9" s="663"/>
       <c r="C9" s="663"/>
@@ -17878,7 +17881,7 @@
       </c>
       <c r="G9" s="386"/>
       <c r="H9" s="692" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="I9" s="693"/>
       <c r="J9" s="693"/>
@@ -17892,7 +17895,7 @@
       <c r="R9" s="693"/>
       <c r="S9" s="694"/>
       <c r="T9" s="695" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="U9" s="664"/>
       <c r="V9" s="664"/>
@@ -17917,7 +17920,7 @@
       </c>
       <c r="G10" s="386"/>
       <c r="H10" s="697" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="I10" s="698"/>
       <c r="J10" s="698"/>
@@ -17954,7 +17957,7 @@
       </c>
       <c r="G11" s="386"/>
       <c r="H11" s="692" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="I11" s="693"/>
       <c r="J11" s="693"/>
@@ -17976,7 +17979,7 @@
       <c r="V11" s="695"/>
       <c r="W11" s="695"/>
       <c r="X11" s="692" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="Y11" s="693"/>
       <c r="Z11" s="693"/>
@@ -17988,14 +17991,14 @@
     </row>
     <row r="12" spans="1:32" ht="23.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A12" s="387" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B12" s="387"/>
       <c r="C12" s="387"/>
       <c r="D12" s="387"/>
       <c r="E12" s="387"/>
       <c r="F12" s="387" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="G12" s="387"/>
       <c r="H12" s="387"/>
@@ -18004,7 +18007,7 @@
       <c r="K12" s="387"/>
       <c r="L12" s="387"/>
       <c r="M12" s="684" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="N12" s="685"/>
       <c r="O12" s="685"/>
@@ -18032,7 +18035,7 @@
       <c r="D13" s="387"/>
       <c r="E13" s="387"/>
       <c r="F13" s="641" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="G13" s="387"/>
       <c r="H13" s="387"/>
@@ -18062,14 +18065,14 @@
     </row>
     <row r="14" spans="1:32" ht="27" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A14" s="150" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B14" s="150"/>
       <c r="C14" s="150"/>
       <c r="D14" s="150"/>
       <c r="E14" s="150"/>
       <c r="F14" s="688" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="G14" s="689"/>
       <c r="H14" s="689"/>
@@ -18078,7 +18081,7 @@
       <c r="K14" s="689"/>
       <c r="L14" s="690"/>
       <c r="M14" s="691" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="N14" s="691"/>
       <c r="O14" s="691"/>
@@ -18107,7 +18110,7 @@
       <c r="C15" s="641"/>
       <c r="D15" s="641"/>
       <c r="E15" s="643" t="s">
-        <v>269</v>
+        <v>430</v>
       </c>
       <c r="F15" s="356"/>
       <c r="G15" s="356"/>
@@ -18183,7 +18186,7 @@
       <c r="D17" s="641"/>
       <c r="E17" s="641" t="str">
         <f>IF(E15=F17,"〇","")</f>
-        <v/>
+        <v>〇</v>
       </c>
       <c r="F17" s="663" t="s">
         <v>266</v>
@@ -18197,7 +18200,7 @@
       </c>
       <c r="L17" s="666"/>
       <c r="M17" s="667" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="N17" s="667"/>
       <c r="O17" s="667"/>
@@ -18210,7 +18213,7 @@
       <c r="T17" s="701"/>
       <c r="U17" s="701"/>
       <c r="V17" s="667" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="W17" s="667"/>
       <c r="X17" s="667"/>
@@ -18236,7 +18239,7 @@
       <c r="I18" s="664"/>
       <c r="J18" s="664"/>
       <c r="K18" s="670" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="L18" s="312"/>
       <c r="M18" s="312"/>
@@ -18248,7 +18251,7 @@
       </c>
       <c r="R18" s="672"/>
       <c r="S18" s="670" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="T18" s="312"/>
       <c r="U18" s="312"/>
@@ -18285,33 +18288,33 @@
       <c r="M19" s="386"/>
       <c r="N19" s="386"/>
       <c r="O19" s="674" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="P19" s="675"/>
       <c r="Q19" s="674" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="R19" s="676"/>
       <c r="S19" s="675"/>
       <c r="T19" s="674" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="U19" s="675"/>
       <c r="V19" s="674" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="W19" s="675"/>
       <c r="X19" s="674" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="Y19" s="676"/>
       <c r="Z19" s="675"/>
       <c r="AA19" s="674" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="AB19" s="675"/>
       <c r="AC19" s="674" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="AD19" s="675"/>
       <c r="AF19" s="57"/>
@@ -18334,7 +18337,7 @@
       <c r="M20" s="386"/>
       <c r="N20" s="386"/>
       <c r="O20" s="390" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="P20" s="391"/>
       <c r="Q20" s="391"/>
@@ -18371,7 +18374,7 @@
       <c r="M21" s="386"/>
       <c r="N21" s="386"/>
       <c r="O21" s="424" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="P21" s="425"/>
       <c r="Q21" s="425"/>
@@ -18511,7 +18514,7 @@
     </row>
     <row r="25" spans="1:32" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A25" s="648" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="B25" s="649"/>
       <c r="C25" s="649"/>
@@ -18528,17 +18531,17 @@
       <c r="N25" s="649"/>
       <c r="O25" s="650"/>
       <c r="P25" s="651" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="Q25" s="652"/>
       <c r="R25" s="653" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="S25" s="654"/>
       <c r="T25" s="654"/>
       <c r="U25" s="655"/>
       <c r="V25" s="656" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="W25" s="657"/>
       <c r="X25" s="657"/>
@@ -18551,7 +18554,7 @@
     </row>
     <row r="26" spans="1:32" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A26" s="648" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="B26" s="649"/>
       <c r="C26" s="649"/>
@@ -18568,17 +18571,17 @@
       <c r="N26" s="649"/>
       <c r="O26" s="650"/>
       <c r="P26" s="651" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="Q26" s="652"/>
       <c r="R26" s="653" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="S26" s="654"/>
       <c r="T26" s="654"/>
       <c r="U26" s="655"/>
       <c r="V26" s="656" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="W26" s="657"/>
       <c r="X26" s="657"/>
@@ -18591,7 +18594,7 @@
     </row>
     <row r="27" spans="1:32" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A27" s="648" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="B27" s="649"/>
       <c r="C27" s="649"/>
@@ -18608,17 +18611,17 @@
       <c r="N27" s="649"/>
       <c r="O27" s="650"/>
       <c r="P27" s="651" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="Q27" s="652"/>
       <c r="R27" s="653" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="S27" s="654"/>
       <c r="T27" s="654"/>
       <c r="U27" s="655"/>
       <c r="V27" s="656" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="W27" s="657"/>
       <c r="X27" s="657"/>
@@ -18631,7 +18634,7 @@
     </row>
     <row r="28" spans="1:32" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A28" s="648" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B28" s="649"/>
       <c r="C28" s="649"/>
@@ -18648,17 +18651,17 @@
       <c r="N28" s="649"/>
       <c r="O28" s="650"/>
       <c r="P28" s="651" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="Q28" s="652"/>
       <c r="R28" s="653" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="S28" s="654"/>
       <c r="T28" s="654"/>
       <c r="U28" s="655"/>
       <c r="V28" s="656" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="W28" s="657"/>
       <c r="X28" s="657"/>
@@ -18671,7 +18674,7 @@
     </row>
     <row r="29" spans="1:32" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A29" s="648" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="B29" s="649"/>
       <c r="C29" s="649"/>
@@ -18688,17 +18691,17 @@
       <c r="N29" s="649"/>
       <c r="O29" s="650"/>
       <c r="P29" s="651" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="Q29" s="652"/>
       <c r="R29" s="653" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="S29" s="654"/>
       <c r="T29" s="654"/>
       <c r="U29" s="655"/>
       <c r="V29" s="656" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="W29" s="657"/>
       <c r="X29" s="657"/>
@@ -19218,21 +19221,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="ドキュメント" ma:contentTypeID="0x010100DE08D44C4358D248A1D08AC8EC8F883B" ma:contentTypeVersion="7" ma:contentTypeDescription="新しいドキュメントを作成します。" ma:contentTypeScope="" ma:versionID="0c8c780510a68c3a39b9039e80410782">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="b691d897-b475-4766-a02f-f4dec49257bd" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9f62a948b310012e1acfd4d77715b87b" ns3:_="">
     <xsd:import namespace="b691d897-b475-4766-a02f-f4dec49257bd"/>
@@ -19396,31 +19384,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E7CD4F1C-447C-4836-AA3F-EAD6FD4ADB25}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C4247B6C-E85F-4ED7-83D9-5DADC5669885}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="b691d897-b475-4766-a02f-f4dec49257bd"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B4C2FACF-02B9-4DDD-8A28-3352238C76AD}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -19436,4 +19415,28 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E7CD4F1C-447C-4836-AA3F-EAD6FD4ADB25}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C4247B6C-E85F-4ED7-83D9-5DADC5669885}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="b691d897-b475-4766-a02f-f4dec49257bd"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>